<commit_message>
4 fichiers avec mes corrections
</commit_message>
<xml_diff>
--- a/comptages/report/template_yearly.xlsx
+++ b/comptages/report/template_yearly.xlsx
@@ -933,7 +933,7 @@
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="0.00%&quot;       &quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1068,6 +1068,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2264,7 +2270,7 @@
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="82" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="441">
+  <cellXfs count="444">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3299,6 +3305,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="83" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="83" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -15980,27 +15989,27 @@
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
-      <c r="C9" s="430" t="str">
+      <c r="C9" s="433" t="str">
         <f>CV_H!C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D9" s="430"/>
-      <c r="E9" s="430"/>
-      <c r="F9" s="431" t="str">
+      <c r="D9" s="433"/>
+      <c r="E9" s="433"/>
+      <c r="F9" s="434" t="str">
         <f>CV_H!F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G9" s="431"/>
-      <c r="H9" s="432" t="str">
+      <c r="G9" s="434"/>
+      <c r="H9" s="435" t="str">
         <f>CV_H!H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I9" s="432"/>
-      <c r="J9" s="423" t="str">
+      <c r="I9" s="435"/>
+      <c r="J9" s="426" t="str">
         <f>CV_H!J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K9" s="423"/>
+      <c r="K9" s="426"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
@@ -16118,28 +16127,28 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="425" t="s">
+      <c r="A14" s="428" t="s">
         <v>223</v>
       </c>
-      <c r="B14" s="425"/>
-      <c r="C14" s="425"/>
-      <c r="D14" s="425"/>
-      <c r="E14" s="425"/>
-      <c r="F14" s="425"/>
-      <c r="G14" s="425"/>
-      <c r="H14" s="425"/>
-      <c r="I14" s="425"/>
-      <c r="J14" s="425"/>
-      <c r="K14" s="425"/>
+      <c r="B14" s="428"/>
+      <c r="C14" s="428"/>
+      <c r="D14" s="428"/>
+      <c r="E14" s="428"/>
+      <c r="F14" s="428"/>
+      <c r="G14" s="428"/>
+      <c r="H14" s="428"/>
+      <c r="I14" s="428"/>
+      <c r="J14" s="428"/>
+      <c r="K14" s="428"/>
     </row>
     <row r="32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="424" t="s">
+      <c r="A33" s="427" t="s">
         <v>204</v>
       </c>
-      <c r="B33" s="424"/>
-      <c r="C33" s="424"/>
-      <c r="D33" s="424"/>
+      <c r="B33" s="427"/>
+      <c r="C33" s="427"/>
+      <c r="D33" s="427"/>
       <c r="E33" s="39"/>
       <c r="F33"/>
       <c r="G33"/>
@@ -16828,27 +16837,27 @@
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
-      <c r="C9" s="430" t="str">
+      <c r="C9" s="433" t="str">
         <f>CV_H!C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D9" s="430"/>
-      <c r="E9" s="430"/>
-      <c r="F9" s="431" t="str">
+      <c r="D9" s="433"/>
+      <c r="E9" s="433"/>
+      <c r="F9" s="434" t="str">
         <f>CV_H!F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G9" s="431"/>
-      <c r="H9" s="432" t="str">
+      <c r="G9" s="434"/>
+      <c r="H9" s="435" t="str">
         <f>CV_H!H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I9" s="432"/>
-      <c r="J9" s="423" t="str">
+      <c r="I9" s="435"/>
+      <c r="J9" s="426" t="str">
         <f>CV_H!J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K9" s="423"/>
+      <c r="K9" s="426"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
@@ -16966,34 +16975,34 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="425" t="s">
+      <c r="A15" s="428" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="425"/>
-      <c r="C15" s="425"/>
-      <c r="D15" s="425"/>
-      <c r="E15" s="425"/>
-      <c r="F15" s="425"/>
-      <c r="G15" s="425"/>
-      <c r="H15" s="425"/>
-      <c r="I15" s="425"/>
-      <c r="J15" s="425"/>
-      <c r="K15" s="425"/>
+      <c r="B15" s="428"/>
+      <c r="C15" s="428"/>
+      <c r="D15" s="428"/>
+      <c r="E15" s="428"/>
+      <c r="F15" s="428"/>
+      <c r="G15" s="428"/>
+      <c r="H15" s="428"/>
+      <c r="I15" s="428"/>
+      <c r="J15" s="428"/>
+      <c r="K15" s="428"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="425" t="s">
+      <c r="A37" s="428" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="425"/>
-      <c r="C37" s="425"/>
-      <c r="D37" s="425"/>
-      <c r="E37" s="425"/>
-      <c r="F37" s="425"/>
-      <c r="G37" s="425"/>
-      <c r="H37" s="425"/>
-      <c r="I37" s="425"/>
-      <c r="J37" s="425"/>
-      <c r="K37" s="425"/>
+      <c r="B37" s="428"/>
+      <c r="C37" s="428"/>
+      <c r="D37" s="428"/>
+      <c r="E37" s="428"/>
+      <c r="F37" s="428"/>
+      <c r="G37" s="428"/>
+      <c r="H37" s="428"/>
+      <c r="I37" s="428"/>
+      <c r="J37" s="428"/>
+      <c r="K37" s="428"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="e">
@@ -17146,21 +17155,21 @@
       <c r="I10" s="66"/>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="434" t="str">
+      <c r="B11" s="437" t="str">
         <f>"Distrubution des classes SWISS7 par tranche horaire  -  Cumul annuel"</f>
         <v>Distrubution des classes SWISS7 par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C11" s="434"/>
-      <c r="D11" s="434"/>
-      <c r="E11" s="434"/>
-      <c r="F11" s="434"/>
-      <c r="G11" s="434"/>
-      <c r="H11" s="434"/>
+      <c r="C11" s="437"/>
+      <c r="D11" s="437"/>
+      <c r="E11" s="437"/>
+      <c r="F11" s="437"/>
+      <c r="G11" s="437"/>
+      <c r="H11" s="437"/>
       <c r="I11" s="229"/>
       <c r="J11" s="230" t="s">
         <v>130</v>
       </c>
-      <c r="K11" s="435" t="s">
+      <c r="K11" s="438" t="s">
         <v>137</v>
       </c>
     </row>
@@ -17193,7 +17202,7 @@
       <c r="J12" s="234" t="s">
         <v>126</v>
       </c>
-      <c r="K12" s="435"/>
+      <c r="K12" s="438"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="235" t="s">
@@ -18327,22 +18336,22 @@
     </row>
     <row r="43" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="B43" s="434" t="str">
+      <c r="B43" s="437" t="str">
         <f>B11</f>
         <v>Distrubution des classes SWISS7 par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C43" s="434"/>
-      <c r="D43" s="434"/>
-      <c r="E43" s="434"/>
-      <c r="F43" s="434"/>
-      <c r="G43" s="434"/>
-      <c r="H43" s="434"/>
+      <c r="C43" s="437"/>
+      <c r="D43" s="437"/>
+      <c r="E43" s="437"/>
+      <c r="F43" s="437"/>
+      <c r="G43" s="437"/>
+      <c r="H43" s="437"/>
       <c r="I43" s="229"/>
       <c r="J43" s="230" t="str">
         <f>J11</f>
         <v>THM</v>
       </c>
-      <c r="K43" s="435" t="str">
+      <c r="K43" s="438" t="str">
         <f>K11</f>
         <v>Part du TJM</v>
       </c>
@@ -18383,7 +18392,7 @@
       <c r="J44" s="234" t="s">
         <v>126</v>
       </c>
-      <c r="K44" s="435"/>
+      <c r="K44" s="438"/>
     </row>
     <row r="45" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="235" t="s">
@@ -19558,14 +19567,14 @@
       <c r="C76" s="275"/>
       <c r="D76" s="275"/>
       <c r="E76" s="275"/>
-      <c r="F76" s="436" t="s">
+      <c r="F76" s="439" t="s">
         <v>155</v>
       </c>
-      <c r="G76" s="436"/>
-      <c r="H76" s="436"/>
-      <c r="I76" s="436"/>
-      <c r="J76" s="436"/>
-      <c r="K76" s="436"/>
+      <c r="G76" s="439"/>
+      <c r="H76" s="439"/>
+      <c r="I76" s="439"/>
+      <c r="J76" s="439"/>
+      <c r="K76" s="439"/>
       <c r="L76" s="274"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
@@ -19788,17 +19797,17 @@
     </row>
     <row r="11" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I11" s="278"/>
-      <c r="J11" s="437" t="s">
+      <c r="J11" s="440" t="s">
         <v>123</v>
       </c>
-      <c r="K11" s="438" t="s">
+      <c r="K11" s="441" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I12" s="245"/>
-      <c r="J12" s="437"/>
-      <c r="K12" s="438"/>
+      <c r="J12" s="440"/>
+      <c r="K12" s="441"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I13" s="245"/>
@@ -20210,18 +20219,18 @@
     <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I46" s="298"/>
-      <c r="J46" s="437" t="s">
+      <c r="J46" s="440" t="s">
         <v>123</v>
       </c>
-      <c r="K46" s="438" t="str">
+      <c r="K46" s="441" t="str">
         <f>K11</f>
         <v>Part du TJM</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I47" s="299"/>
-      <c r="J47" s="437"/>
-      <c r="K47" s="438"/>
+      <c r="J47" s="440"/>
+      <c r="K47" s="441"/>
     </row>
     <row r="48" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I48" s="299"/>
@@ -20777,24 +20786,24 @@
       <c r="L10" s="66"/>
     </row>
     <row r="11" spans="1:14" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="434" t="str">
+      <c r="B11" s="437" t="str">
         <f>"Distrubution des classes SWISS10 par tranche horaire  -  Cumul annuel"</f>
         <v>Distrubution des classes SWISS10 par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C11" s="434"/>
-      <c r="D11" s="434"/>
-      <c r="E11" s="434"/>
-      <c r="F11" s="434"/>
-      <c r="G11" s="434"/>
-      <c r="H11" s="434"/>
-      <c r="I11" s="434"/>
-      <c r="J11" s="434"/>
-      <c r="K11" s="434"/>
+      <c r="C11" s="437"/>
+      <c r="D11" s="437"/>
+      <c r="E11" s="437"/>
+      <c r="F11" s="437"/>
+      <c r="G11" s="437"/>
+      <c r="H11" s="437"/>
+      <c r="I11" s="437"/>
+      <c r="J11" s="437"/>
+      <c r="K11" s="437"/>
       <c r="L11" s="301"/>
       <c r="M11" s="230" t="s">
         <v>130</v>
       </c>
-      <c r="N11" s="438" t="s">
+      <c r="N11" s="441" t="s">
         <v>137</v>
       </c>
     </row>
@@ -20836,7 +20845,7 @@
       <c r="M12" s="234" t="s">
         <v>126</v>
       </c>
-      <c r="N12" s="438"/>
+      <c r="N12" s="441"/>
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="235" t="s">
@@ -22320,24 +22329,24 @@
     </row>
     <row r="43" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="B43" s="434" t="str">
+      <c r="B43" s="437" t="str">
         <f>B11</f>
         <v>Distrubution des classes SWISS10 par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C43" s="434"/>
-      <c r="D43" s="434"/>
-      <c r="E43" s="434"/>
-      <c r="F43" s="434"/>
-      <c r="G43" s="434"/>
-      <c r="H43" s="434"/>
-      <c r="I43" s="434"/>
-      <c r="J43" s="434"/>
-      <c r="K43" s="434"/>
+      <c r="C43" s="437"/>
+      <c r="D43" s="437"/>
+      <c r="E43" s="437"/>
+      <c r="F43" s="437"/>
+      <c r="G43" s="437"/>
+      <c r="H43" s="437"/>
+      <c r="I43" s="437"/>
+      <c r="J43" s="437"/>
+      <c r="K43" s="437"/>
       <c r="L43" s="301"/>
       <c r="M43" s="230" t="s">
         <v>130</v>
       </c>
-      <c r="N43" s="438" t="str">
+      <c r="N43" s="441" t="str">
         <f>N11</f>
         <v>Part du TJM</v>
       </c>
@@ -22390,7 +22399,7 @@
       <c r="M44" s="234" t="s">
         <v>126</v>
       </c>
-      <c r="N44" s="438"/>
+      <c r="N44" s="441"/>
     </row>
     <row r="45" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="235" t="s">
@@ -24146,17 +24155,17 @@
     </row>
     <row r="11" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L11" s="298"/>
-      <c r="M11" s="437" t="s">
+      <c r="M11" s="440" t="s">
         <v>123</v>
       </c>
-      <c r="N11" s="438" t="s">
+      <c r="N11" s="441" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L12" s="299"/>
-      <c r="M12" s="437"/>
-      <c r="N12" s="438"/>
+      <c r="M12" s="440"/>
+      <c r="N12" s="441"/>
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L13" s="244"/>
@@ -24616,18 +24625,18 @@
     <row r="45" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L46" s="298"/>
-      <c r="M46" s="437" t="s">
+      <c r="M46" s="440" t="s">
         <v>123</v>
       </c>
-      <c r="N46" s="438" t="str">
+      <c r="N46" s="441" t="str">
         <f>N11</f>
         <v>Part du TJM</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L47" s="299"/>
-      <c r="M47" s="437"/>
-      <c r="N47" s="438"/>
+      <c r="M47" s="440"/>
+      <c r="N47" s="441"/>
     </row>
     <row r="48" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L48" s="244"/>
@@ -25232,20 +25241,20 @@
       <c r="H10" s="66"/>
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="434" t="str">
+      <c r="B11" s="437" t="str">
         <f>"Distrubution des classes EUR6 par tranche horaire  -  Cumul annuel"</f>
         <v>Distrubution des classes EUR6 par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C11" s="434"/>
-      <c r="D11" s="434"/>
-      <c r="E11" s="434"/>
-      <c r="F11" s="434"/>
-      <c r="G11" s="434"/>
+      <c r="C11" s="437"/>
+      <c r="D11" s="437"/>
+      <c r="E11" s="437"/>
+      <c r="F11" s="437"/>
+      <c r="G11" s="437"/>
       <c r="H11" s="229"/>
       <c r="I11" s="230" t="s">
         <v>130</v>
       </c>
-      <c r="J11" s="435" t="s">
+      <c r="J11" s="438" t="s">
         <v>137</v>
       </c>
     </row>
@@ -25275,7 +25284,7 @@
       <c r="I12" s="234" t="s">
         <v>126</v>
       </c>
-      <c r="J12" s="435"/>
+      <c r="J12" s="438"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="235" t="s">
@@ -26300,21 +26309,21 @@
     </row>
     <row r="43" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="434" t="str">
+      <c r="B43" s="437" t="str">
         <f>B11</f>
         <v>Distrubution des classes EUR6 par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C43" s="434"/>
-      <c r="D43" s="434"/>
-      <c r="E43" s="434"/>
-      <c r="F43" s="434"/>
-      <c r="G43" s="434"/>
+      <c r="C43" s="437"/>
+      <c r="D43" s="437"/>
+      <c r="E43" s="437"/>
+      <c r="F43" s="437"/>
+      <c r="G43" s="437"/>
       <c r="H43" s="229"/>
       <c r="I43" s="230" t="str">
         <f>I11</f>
         <v>THM</v>
       </c>
-      <c r="J43" s="435" t="str">
+      <c r="J43" s="438" t="str">
         <f>J11</f>
         <v>Part du TJM</v>
       </c>
@@ -26351,7 +26360,7 @@
       <c r="I44" s="234" t="s">
         <v>126</v>
       </c>
-      <c r="J44" s="435"/>
+      <c r="J44" s="438"/>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="235" t="s">
@@ -27404,20 +27413,20 @@
       <c r="K75" s="274"/>
     </row>
     <row r="76" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="439" t="s">
+      <c r="A76" s="442" t="s">
         <v>217</v>
       </c>
-      <c r="B76" s="439"/>
-      <c r="C76" s="439"/>
-      <c r="D76" s="439"/>
+      <c r="B76" s="442"/>
+      <c r="C76" s="442"/>
+      <c r="D76" s="442"/>
       <c r="E76" s="275"/>
-      <c r="F76" s="436" t="s">
+      <c r="F76" s="439" t="s">
         <v>218</v>
       </c>
-      <c r="G76" s="436"/>
-      <c r="H76" s="436"/>
-      <c r="I76" s="436"/>
-      <c r="J76" s="436"/>
+      <c r="G76" s="439"/>
+      <c r="H76" s="439"/>
+      <c r="I76" s="439"/>
+      <c r="J76" s="439"/>
       <c r="K76" s="274"/>
     </row>
   </sheetData>
@@ -27585,17 +27594,17 @@
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H11" s="278"/>
-      <c r="I11" s="437" t="s">
+      <c r="I11" s="440" t="s">
         <v>123</v>
       </c>
-      <c r="J11" s="438" t="s">
+      <c r="J11" s="441" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H12" s="245"/>
-      <c r="I12" s="437"/>
-      <c r="J12" s="438"/>
+      <c r="I12" s="440"/>
+      <c r="J12" s="441"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H13" s="245"/>
@@ -27991,18 +28000,18 @@
     <row r="45" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H46" s="298"/>
-      <c r="I46" s="437" t="s">
+      <c r="I46" s="440" t="s">
         <v>123</v>
       </c>
-      <c r="J46" s="438" t="str">
+      <c r="J46" s="441" t="str">
         <f>J11</f>
         <v>Part du TJM</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H47" s="299"/>
-      <c r="I47" s="437"/>
-      <c r="J47" s="438"/>
+      <c r="I47" s="440"/>
+      <c r="J47" s="441"/>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H48" s="299"/>
@@ -28536,38 +28545,38 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="440"/>
-      <c r="B11" s="440"/>
-      <c r="C11" s="440"/>
-      <c r="D11" s="440"/>
-      <c r="E11" s="440"/>
-      <c r="F11" s="440"/>
-      <c r="G11" s="440"/>
-      <c r="H11" s="440"/>
-      <c r="I11" s="440"/>
-      <c r="J11" s="440"/>
-      <c r="K11" s="440"/>
-      <c r="L11" s="440"/>
-      <c r="M11" s="440"/>
-      <c r="N11" s="440"/>
-      <c r="O11" s="440"/>
+      <c r="A11" s="443"/>
+      <c r="B11" s="443"/>
+      <c r="C11" s="443"/>
+      <c r="D11" s="443"/>
+      <c r="E11" s="443"/>
+      <c r="F11" s="443"/>
+      <c r="G11" s="443"/>
+      <c r="H11" s="443"/>
+      <c r="I11" s="443"/>
+      <c r="J11" s="443"/>
+      <c r="K11" s="443"/>
+      <c r="L11" s="443"/>
+      <c r="M11" s="443"/>
+      <c r="N11" s="443"/>
+      <c r="O11" s="443"/>
     </row>
     <row r="12" spans="1:15" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="434" t="str">
+      <c r="B12" s="437" t="str">
         <f>"Distribution de la Vitesse par tranche horaire  -  Cumul annuel"</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C12" s="434"/>
-      <c r="D12" s="434"/>
-      <c r="E12" s="434"/>
-      <c r="F12" s="434"/>
-      <c r="G12" s="434"/>
-      <c r="H12" s="434"/>
-      <c r="I12" s="434"/>
-      <c r="J12" s="434"/>
-      <c r="K12" s="434"/>
-      <c r="L12" s="434"/>
-      <c r="M12" s="434"/>
+      <c r="C12" s="437"/>
+      <c r="D12" s="437"/>
+      <c r="E12" s="437"/>
+      <c r="F12" s="437"/>
+      <c r="G12" s="437"/>
+      <c r="H12" s="437"/>
+      <c r="I12" s="437"/>
+      <c r="J12" s="437"/>
+      <c r="K12" s="437"/>
+      <c r="L12" s="437"/>
+      <c r="M12" s="437"/>
       <c r="N12" s="229"/>
       <c r="O12" s="230" t="s">
         <v>130</v>
@@ -30187,39 +30196,39 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="440"/>
-      <c r="B46" s="440"/>
-      <c r="C46" s="440"/>
-      <c r="D46" s="440"/>
-      <c r="E46" s="440"/>
-      <c r="F46" s="440"/>
-      <c r="G46" s="440"/>
-      <c r="H46" s="440"/>
-      <c r="I46" s="440"/>
-      <c r="J46" s="440"/>
-      <c r="K46" s="440"/>
-      <c r="L46" s="440"/>
-      <c r="M46" s="440"/>
-      <c r="N46" s="440"/>
-      <c r="O46" s="440"/>
+      <c r="A46" s="443"/>
+      <c r="B46" s="443"/>
+      <c r="C46" s="443"/>
+      <c r="D46" s="443"/>
+      <c r="E46" s="443"/>
+      <c r="F46" s="443"/>
+      <c r="G46" s="443"/>
+      <c r="H46" s="443"/>
+      <c r="I46" s="443"/>
+      <c r="J46" s="443"/>
+      <c r="K46" s="443"/>
+      <c r="L46" s="443"/>
+      <c r="M46" s="443"/>
+      <c r="N46" s="443"/>
+      <c r="O46" s="443"/>
     </row>
     <row r="47" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="434" t="str">
+      <c r="B47" s="437" t="str">
         <f>B12</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C47" s="434"/>
-      <c r="D47" s="434"/>
-      <c r="E47" s="434"/>
-      <c r="F47" s="434"/>
-      <c r="G47" s="434"/>
-      <c r="H47" s="434"/>
-      <c r="I47" s="434"/>
-      <c r="J47" s="434"/>
-      <c r="K47" s="434"/>
-      <c r="L47" s="434"/>
-      <c r="M47" s="434"/>
+      <c r="C47" s="437"/>
+      <c r="D47" s="437"/>
+      <c r="E47" s="437"/>
+      <c r="F47" s="437"/>
+      <c r="G47" s="437"/>
+      <c r="H47" s="437"/>
+      <c r="I47" s="437"/>
+      <c r="J47" s="437"/>
+      <c r="K47" s="437"/>
+      <c r="L47" s="437"/>
+      <c r="M47" s="437"/>
       <c r="N47" s="229"/>
       <c r="O47" s="230" t="str">
         <f>O12</f>
@@ -31983,59 +31992,59 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="440" t="str">
+      <c r="A11" s="443" t="str">
         <f>"Vitesse moyenne = "&amp;INT(U39)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
-      <c r="B11" s="440"/>
-      <c r="C11" s="440"/>
-      <c r="D11" s="440"/>
-      <c r="E11" s="440"/>
-      <c r="F11" s="440"/>
-      <c r="G11" s="440"/>
-      <c r="H11" s="440"/>
-      <c r="I11" s="440"/>
-      <c r="J11" s="440"/>
-      <c r="K11" s="440"/>
-      <c r="L11" s="440"/>
-      <c r="M11" s="440"/>
-      <c r="N11" s="440"/>
-      <c r="O11" s="440"/>
-      <c r="P11" s="440"/>
-      <c r="Q11" s="440"/>
-      <c r="R11" s="440"/>
-      <c r="S11" s="440"/>
-      <c r="T11" s="440"/>
-      <c r="U11" s="440"/>
+      <c r="B11" s="443"/>
+      <c r="C11" s="443"/>
+      <c r="D11" s="443"/>
+      <c r="E11" s="443"/>
+      <c r="F11" s="443"/>
+      <c r="G11" s="443"/>
+      <c r="H11" s="443"/>
+      <c r="I11" s="443"/>
+      <c r="J11" s="443"/>
+      <c r="K11" s="443"/>
+      <c r="L11" s="443"/>
+      <c r="M11" s="443"/>
+      <c r="N11" s="443"/>
+      <c r="O11" s="443"/>
+      <c r="P11" s="443"/>
+      <c r="Q11" s="443"/>
+      <c r="R11" s="443"/>
+      <c r="S11" s="443"/>
+      <c r="T11" s="443"/>
+      <c r="U11" s="443"/>
     </row>
     <row r="12" spans="1:21" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="434" t="str">
+      <c r="B12" s="437" t="str">
         <f>"Distribution de la Vitesse par tranche horaire  -  Cumul annuel"</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C12" s="434"/>
-      <c r="D12" s="434"/>
-      <c r="E12" s="434"/>
-      <c r="F12" s="434"/>
-      <c r="G12" s="434"/>
-      <c r="H12" s="434"/>
-      <c r="I12" s="434"/>
-      <c r="J12" s="434"/>
-      <c r="K12" s="434"/>
-      <c r="L12" s="434"/>
-      <c r="M12" s="434"/>
-      <c r="N12" s="434"/>
+      <c r="C12" s="437"/>
+      <c r="D12" s="437"/>
+      <c r="E12" s="437"/>
+      <c r="F12" s="437"/>
+      <c r="G12" s="437"/>
+      <c r="H12" s="437"/>
+      <c r="I12" s="437"/>
+      <c r="J12" s="437"/>
+      <c r="K12" s="437"/>
+      <c r="L12" s="437"/>
+      <c r="M12" s="437"/>
+      <c r="N12" s="437"/>
       <c r="O12" s="229"/>
       <c r="P12" s="230" t="s">
         <v>130</v>
       </c>
       <c r="Q12" s="301"/>
-      <c r="R12" s="434" t="s">
+      <c r="R12" s="437" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="434"/>
-      <c r="T12" s="434"/>
-      <c r="U12" s="434"/>
+      <c r="S12" s="437"/>
+      <c r="T12" s="437"/>
+      <c r="U12" s="437"/>
     </row>
     <row r="13" spans="1:21" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115" t="s">
@@ -34246,62 +34255,62 @@
       <c r="U45" s="7"/>
     </row>
     <row r="46" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="440" t="str">
+      <c r="A46" s="443" t="str">
         <f>"Vitesse moyenne = "&amp;INT(U74)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
-      <c r="B46" s="440"/>
-      <c r="C46" s="440"/>
-      <c r="D46" s="440"/>
-      <c r="E46" s="440"/>
-      <c r="F46" s="440"/>
-      <c r="G46" s="440"/>
-      <c r="H46" s="440"/>
-      <c r="I46" s="440"/>
-      <c r="J46" s="440"/>
-      <c r="K46" s="440"/>
-      <c r="L46" s="440"/>
-      <c r="M46" s="440"/>
-      <c r="N46" s="440"/>
-      <c r="O46" s="440"/>
-      <c r="P46" s="440"/>
-      <c r="Q46" s="440"/>
-      <c r="R46" s="440"/>
-      <c r="S46" s="440"/>
-      <c r="T46" s="440"/>
-      <c r="U46" s="440"/>
+      <c r="B46" s="443"/>
+      <c r="C46" s="443"/>
+      <c r="D46" s="443"/>
+      <c r="E46" s="443"/>
+      <c r="F46" s="443"/>
+      <c r="G46" s="443"/>
+      <c r="H46" s="443"/>
+      <c r="I46" s="443"/>
+      <c r="J46" s="443"/>
+      <c r="K46" s="443"/>
+      <c r="L46" s="443"/>
+      <c r="M46" s="443"/>
+      <c r="N46" s="443"/>
+      <c r="O46" s="443"/>
+      <c r="P46" s="443"/>
+      <c r="Q46" s="443"/>
+      <c r="R46" s="443"/>
+      <c r="S46" s="443"/>
+      <c r="T46" s="443"/>
+      <c r="U46" s="443"/>
     </row>
     <row r="47" spans="1:21" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="434" t="str">
+      <c r="B47" s="437" t="str">
         <f>B12</f>
         <v>Distribution de la Vitesse par tranche horaire  -  Cumul annuel</v>
       </c>
-      <c r="C47" s="434"/>
-      <c r="D47" s="434"/>
-      <c r="E47" s="434"/>
-      <c r="F47" s="434"/>
-      <c r="G47" s="434"/>
-      <c r="H47" s="434"/>
-      <c r="I47" s="434"/>
-      <c r="J47" s="434"/>
-      <c r="K47" s="434"/>
-      <c r="L47" s="434"/>
-      <c r="M47" s="434"/>
-      <c r="N47" s="434"/>
+      <c r="C47" s="437"/>
+      <c r="D47" s="437"/>
+      <c r="E47" s="437"/>
+      <c r="F47" s="437"/>
+      <c r="G47" s="437"/>
+      <c r="H47" s="437"/>
+      <c r="I47" s="437"/>
+      <c r="J47" s="437"/>
+      <c r="K47" s="437"/>
+      <c r="L47" s="437"/>
+      <c r="M47" s="437"/>
+      <c r="N47" s="437"/>
       <c r="O47" s="229"/>
       <c r="P47" s="230" t="str">
         <f>P12</f>
         <v>THM</v>
       </c>
       <c r="Q47" s="301"/>
-      <c r="R47" s="434" t="str">
+      <c r="R47" s="437" t="str">
         <f>R12</f>
         <v>Vitesses caractéristiques</v>
       </c>
-      <c r="S47" s="434"/>
-      <c r="T47" s="434"/>
-      <c r="U47" s="434"/>
+      <c r="S47" s="437"/>
+      <c r="T47" s="437"/>
+      <c r="U47" s="437"/>
     </row>
     <row r="48" spans="1:21" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="115" t="s">
@@ -36543,9 +36552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:I67"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -36563,8 +36570,8 @@
     <col min="21" max="22" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -41741,18 +41748,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="412" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="Q2" s="410" t="s">
+      <c r="Q2" s="413" t="s">
         <v>264</v>
       </c>
-      <c r="R2" s="411"/>
-      <c r="S2" s="411"/>
-      <c r="T2" s="411"/>
-      <c r="U2" s="412"/>
+      <c r="R2" s="414"/>
+      <c r="S2" s="414"/>
+      <c r="T2" s="414"/>
+      <c r="U2" s="415"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -41801,12 +41808,12 @@
         <v>95</v>
       </c>
       <c r="Q3" s="409"/>
-      <c r="R3" s="410" t="s">
+      <c r="R3" s="413" t="s">
         <v>258</v>
       </c>
-      <c r="S3" s="411"/>
-      <c r="T3" s="411"/>
-      <c r="U3" s="412"/>
+      <c r="S3" s="414"/>
+      <c r="T3" s="414"/>
+      <c r="U3" s="415"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B4" s="8">
@@ -42452,8 +42459,8 @@
     <col min="1" max="19" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>96</v>
       </c>
     </row>
@@ -45603,8 +45610,8 @@
     <col min="1" max="24" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="2"/>
@@ -45619,7 +45626,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1">
+      <c r="B4" s="410">
         <v>0</v>
       </c>
       <c r="C4" s="1">
@@ -45693,7 +45700,7 @@
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="411">
         <v>0</v>
       </c>
       <c r="C5" s="8">
@@ -45779,7 +45786,7 @@
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="411">
         <v>0</v>
       </c>
       <c r="C6" s="8">
@@ -45865,7 +45872,7 @@
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="411">
         <v>0</v>
       </c>
       <c r="C7" s="8">
@@ -45951,7 +45958,7 @@
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="411">
         <v>0</v>
       </c>
       <c r="C8" s="8">
@@ -46037,7 +46044,7 @@
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="411">
         <v>0</v>
       </c>
       <c r="C9" s="8">
@@ -46123,7 +46130,7 @@
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="411">
         <v>0</v>
       </c>
       <c r="C10" s="8">
@@ -46209,7 +46216,7 @@
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="411">
         <v>0</v>
       </c>
       <c r="C11" s="8">
@@ -46295,7 +46302,7 @@
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="411">
         <v>0</v>
       </c>
       <c r="C12" s="8">
@@ -46381,7 +46388,7 @@
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="411">
         <v>0</v>
       </c>
       <c r="C13" s="8">
@@ -46467,7 +46474,7 @@
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="411">
         <v>0</v>
       </c>
       <c r="C14" s="8">
@@ -46553,7 +46560,7 @@
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="411">
         <v>0</v>
       </c>
       <c r="C15" s="8">
@@ -46639,7 +46646,7 @@
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="411">
         <v>0</v>
       </c>
       <c r="C16" s="8">
@@ -46725,7 +46732,7 @@
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="411">
         <v>0</v>
       </c>
       <c r="C17" s="8">
@@ -46811,7 +46818,7 @@
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="411">
         <v>0</v>
       </c>
       <c r="C18" s="8">
@@ -46897,7 +46904,7 @@
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="411">
         <v>0</v>
       </c>
       <c r="C19" s="8">
@@ -46983,7 +46990,7 @@
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="411">
         <v>0</v>
       </c>
       <c r="C20" s="8">
@@ -47069,7 +47076,7 @@
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="411">
         <v>0</v>
       </c>
       <c r="C21" s="8">
@@ -47155,7 +47162,7 @@
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="411">
         <v>0</v>
       </c>
       <c r="C22" s="8">
@@ -47241,7 +47248,7 @@
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="411">
         <v>0</v>
       </c>
       <c r="C23" s="8">
@@ -47327,7 +47334,7 @@
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="411">
         <v>0</v>
       </c>
       <c r="C24" s="8">
@@ -47413,7 +47420,7 @@
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="411">
         <v>0</v>
       </c>
       <c r="C25" s="8">
@@ -47499,7 +47506,7 @@
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="411">
         <v>0</v>
       </c>
       <c r="C26" s="8">
@@ -47585,7 +47592,7 @@
       <c r="A27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="411">
         <v>0</v>
       </c>
       <c r="C27" s="8">
@@ -47671,7 +47678,7 @@
       <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="411">
         <v>0</v>
       </c>
       <c r="C28" s="8">
@@ -47757,7 +47764,7 @@
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="410">
         <f t="shared" ref="B29:L29" si="13">SUM(B5:B28)</f>
         <v>0</v>
       </c>
@@ -47821,7 +47828,7 @@
       </c>
     </row>
     <row r="32" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1">
+      <c r="B32" s="410">
         <v>0</v>
       </c>
       <c r="C32" s="1">
@@ -47895,7 +47902,7 @@
       <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="411">
         <v>0</v>
       </c>
       <c r="C33" s="8">
@@ -47981,7 +47988,7 @@
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="411">
         <v>0</v>
       </c>
       <c r="C34" s="8">
@@ -48067,7 +48074,7 @@
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="411">
         <v>0</v>
       </c>
       <c r="C35" s="8">
@@ -48153,7 +48160,7 @@
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="411">
         <v>0</v>
       </c>
       <c r="C36" s="8">
@@ -48239,7 +48246,7 @@
       <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="411">
         <v>0</v>
       </c>
       <c r="C37" s="8">
@@ -48325,7 +48332,7 @@
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="411">
         <v>0</v>
       </c>
       <c r="C38" s="8">
@@ -48411,7 +48418,7 @@
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="411">
         <v>0</v>
       </c>
       <c r="C39" s="8">
@@ -48497,7 +48504,7 @@
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="411">
         <v>0</v>
       </c>
       <c r="C40" s="8">
@@ -48583,7 +48590,7 @@
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="411">
         <v>0</v>
       </c>
       <c r="C41" s="8">
@@ -48669,7 +48676,7 @@
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="411">
         <v>0</v>
       </c>
       <c r="C42" s="8">
@@ -48755,7 +48762,7 @@
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="411">
         <v>0</v>
       </c>
       <c r="C43" s="8">
@@ -48841,7 +48848,7 @@
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="411">
         <v>0</v>
       </c>
       <c r="C44" s="8">
@@ -48927,7 +48934,7 @@
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="411">
         <v>0</v>
       </c>
       <c r="C45" s="8">
@@ -49013,7 +49020,7 @@
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="411">
         <v>0</v>
       </c>
       <c r="C46" s="8">
@@ -49099,7 +49106,7 @@
       <c r="A47" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="411">
         <v>0</v>
       </c>
       <c r="C47" s="8">
@@ -49185,7 +49192,7 @@
       <c r="A48" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="411">
         <v>0</v>
       </c>
       <c r="C48" s="8">
@@ -49271,7 +49278,7 @@
       <c r="A49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="411">
         <v>0</v>
       </c>
       <c r="C49" s="8">
@@ -49357,7 +49364,7 @@
       <c r="A50" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="411">
         <v>0</v>
       </c>
       <c r="C50" s="8">
@@ -49443,7 +49450,7 @@
       <c r="A51" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="411">
         <v>0</v>
       </c>
       <c r="C51" s="8">
@@ -49529,7 +49536,7 @@
       <c r="A52" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="411">
         <v>0</v>
       </c>
       <c r="C52" s="8">
@@ -49615,7 +49622,7 @@
       <c r="A53" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="411">
         <v>0</v>
       </c>
       <c r="C53" s="8">
@@ -49701,7 +49708,7 @@
       <c r="A54" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="411">
         <v>0</v>
       </c>
       <c r="C54" s="8">
@@ -49787,7 +49794,7 @@
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="411">
         <v>0</v>
       </c>
       <c r="C55" s="8">
@@ -49873,7 +49880,7 @@
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="411">
         <v>0</v>
       </c>
       <c r="C56" s="8">
@@ -49959,7 +49966,7 @@
       <c r="A57" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="410">
         <f t="shared" ref="B57:L57" si="27">SUM(B33:B56)</f>
         <v>0</v>
       </c>
@@ -51573,7 +51580,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -51699,41 +51706,41 @@
     <row r="11" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:30" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="413" t="s">
+      <c r="B12" s="416" t="s">
         <v>219</v>
       </c>
-      <c r="C12" s="413"/>
-      <c r="D12" s="413"/>
-      <c r="E12" s="413"/>
-      <c r="F12" s="413"/>
-      <c r="G12" s="413"/>
-      <c r="H12" s="413"/>
-      <c r="I12" s="413"/>
-      <c r="J12" s="413"/>
+      <c r="C12" s="416"/>
+      <c r="D12" s="416"/>
+      <c r="E12" s="416"/>
+      <c r="F12" s="416"/>
+      <c r="G12" s="416"/>
+      <c r="H12" s="416"/>
+      <c r="I12" s="416"/>
+      <c r="J12" s="416"/>
       <c r="K12" s="146"/>
-      <c r="L12" s="413" t="s">
+      <c r="L12" s="416" t="s">
         <v>220</v>
       </c>
-      <c r="M12" s="413"/>
-      <c r="N12" s="413"/>
-      <c r="O12" s="413"/>
-      <c r="P12" s="413"/>
-      <c r="Q12" s="413"/>
-      <c r="R12" s="413"/>
-      <c r="S12" s="413"/>
-      <c r="T12" s="413"/>
+      <c r="M12" s="416"/>
+      <c r="N12" s="416"/>
+      <c r="O12" s="416"/>
+      <c r="P12" s="416"/>
+      <c r="Q12" s="416"/>
+      <c r="R12" s="416"/>
+      <c r="S12" s="416"/>
+      <c r="T12" s="416"/>
       <c r="U12" s="146"/>
-      <c r="V12" s="413" t="s">
+      <c r="V12" s="416" t="s">
         <v>221</v>
       </c>
-      <c r="W12" s="413"/>
-      <c r="X12" s="413"/>
-      <c r="Y12" s="413"/>
-      <c r="Z12" s="413"/>
-      <c r="AA12" s="413"/>
-      <c r="AB12" s="413"/>
-      <c r="AC12" s="413"/>
-      <c r="AD12" s="413"/>
+      <c r="W12" s="416"/>
+      <c r="X12" s="416"/>
+      <c r="Y12" s="416"/>
+      <c r="Z12" s="416"/>
+      <c r="AA12" s="416"/>
+      <c r="AB12" s="416"/>
+      <c r="AC12" s="416"/>
+      <c r="AD12" s="416"/>
     </row>
     <row r="13" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="147" t="s">
@@ -54888,36 +54895,36 @@
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="414" t="s">
+      <c r="C9" s="417" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="415"/>
-      <c r="E9" s="415"/>
-      <c r="F9" s="415"/>
-      <c r="G9" s="415"/>
-      <c r="H9" s="415"/>
-      <c r="I9" s="415"/>
-      <c r="J9" s="415"/>
-      <c r="K9" s="416"/>
+      <c r="D9" s="418"/>
+      <c r="E9" s="418"/>
+      <c r="F9" s="418"/>
+      <c r="G9" s="418"/>
+      <c r="H9" s="418"/>
+      <c r="I9" s="418"/>
+      <c r="J9" s="418"/>
+      <c r="K9" s="419"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="417" t="s">
+      <c r="C10" s="420" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="418"/>
-      <c r="E10" s="419"/>
-      <c r="F10" s="420" t="s">
+      <c r="D10" s="421"/>
+      <c r="E10" s="422"/>
+      <c r="F10" s="423" t="s">
         <v>107</v>
       </c>
-      <c r="G10" s="419"/>
-      <c r="H10" s="420" t="s">
+      <c r="G10" s="422"/>
+      <c r="H10" s="423" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="419"/>
-      <c r="J10" s="421" t="s">
+      <c r="I10" s="422"/>
+      <c r="J10" s="424" t="s">
         <v>109</v>
       </c>
-      <c r="K10" s="422"/>
+      <c r="K10" s="425"/>
     </row>
     <row r="11" spans="1:12" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
@@ -55584,40 +55591,40 @@
       <c r="K39" s="382"/>
     </row>
     <row r="40" spans="1:12" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="414" t="s">
+      <c r="C40" s="417" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="415"/>
-      <c r="E40" s="415"/>
-      <c r="F40" s="415"/>
-      <c r="G40" s="415"/>
-      <c r="H40" s="415"/>
-      <c r="I40" s="415"/>
-      <c r="J40" s="415"/>
-      <c r="K40" s="416"/>
+      <c r="D40" s="418"/>
+      <c r="E40" s="418"/>
+      <c r="F40" s="418"/>
+      <c r="G40" s="418"/>
+      <c r="H40" s="418"/>
+      <c r="I40" s="418"/>
+      <c r="J40" s="418"/>
+      <c r="K40" s="419"/>
     </row>
     <row r="41" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="417" t="str">
+      <c r="C41" s="420" t="str">
         <f>C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D41" s="418"/>
-      <c r="E41" s="419"/>
-      <c r="F41" s="420" t="str">
+      <c r="D41" s="421"/>
+      <c r="E41" s="422"/>
+      <c r="F41" s="423" t="str">
         <f>F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G41" s="419"/>
-      <c r="H41" s="420" t="str">
+      <c r="G41" s="422"/>
+      <c r="H41" s="423" t="str">
         <f>H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I41" s="419"/>
-      <c r="J41" s="421" t="str">
+      <c r="I41" s="422"/>
+      <c r="J41" s="424" t="str">
         <f t="shared" ref="J41:J47" si="5">J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K41" s="422"/>
+      <c r="K41" s="425"/>
     </row>
     <row r="42" spans="1:12" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C42" s="20" t="str">
@@ -56236,27 +56243,27 @@
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
-      <c r="C9" s="430" t="str">
+      <c r="C9" s="433" t="str">
         <f>CV_H!C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D9" s="430"/>
-      <c r="E9" s="430"/>
-      <c r="F9" s="431" t="str">
+      <c r="D9" s="433"/>
+      <c r="E9" s="433"/>
+      <c r="F9" s="434" t="str">
         <f>CV_H!F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G9" s="431"/>
-      <c r="H9" s="432" t="str">
+      <c r="G9" s="434"/>
+      <c r="H9" s="435" t="str">
         <f>CV_H!H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I9" s="432"/>
-      <c r="J9" s="423" t="str">
+      <c r="I9" s="435"/>
+      <c r="J9" s="426" t="str">
         <f>CV_H!J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K9" s="423"/>
+      <c r="K9" s="426"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
@@ -56374,28 +56381,28 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="425" t="s">
+      <c r="A14" s="428" t="s">
         <v>200</v>
       </c>
-      <c r="B14" s="425"/>
-      <c r="C14" s="425"/>
-      <c r="D14" s="425"/>
-      <c r="E14" s="425"/>
-      <c r="F14" s="425"/>
-      <c r="G14" s="425"/>
-      <c r="H14" s="425"/>
-      <c r="I14" s="425"/>
-      <c r="J14" s="425"/>
-      <c r="K14" s="425"/>
+      <c r="B14" s="428"/>
+      <c r="C14" s="428"/>
+      <c r="D14" s="428"/>
+      <c r="E14" s="428"/>
+      <c r="F14" s="428"/>
+      <c r="G14" s="428"/>
+      <c r="H14" s="428"/>
+      <c r="I14" s="428"/>
+      <c r="J14" s="428"/>
+      <c r="K14" s="428"/>
     </row>
     <row r="32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="424" t="s">
+      <c r="A33" s="427" t="s">
         <v>201</v>
       </c>
-      <c r="B33" s="424"/>
-      <c r="C33" s="424"/>
-      <c r="D33" s="424"/>
+      <c r="B33" s="427"/>
+      <c r="C33" s="427"/>
+      <c r="D33" s="427"/>
       <c r="E33" s="39"/>
       <c r="G33"/>
       <c r="H33"/>
@@ -56636,12 +56643,12 @@
         <f>CV_C!I23</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F44" s="428" t="s">
+      <c r="F44" s="431" t="s">
         <v>224</v>
       </c>
-      <c r="G44" s="429"/>
-      <c r="H44" s="429"/>
-      <c r="I44" s="423"/>
+      <c r="G44" s="432"/>
+      <c r="H44" s="432"/>
+      <c r="I44" s="426"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
@@ -56661,8 +56668,8 @@
         <f>CV_C!I24</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F45" s="426"/>
-      <c r="G45" s="427"/>
+      <c r="F45" s="429"/>
+      <c r="G45" s="430"/>
       <c r="H45" s="394" t="s">
         <v>225</v>
       </c>
@@ -56711,10 +56718,10 @@
         <f>CV_C!I26</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F47" s="426" t="s">
+      <c r="F47" s="429" t="s">
         <v>227</v>
       </c>
-      <c r="G47" s="427"/>
+      <c r="G47" s="430"/>
       <c r="H47" s="243" t="s">
         <v>228</v>
       </c>
@@ -56738,10 +56745,10 @@
         <f>CV_C!I27</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F48" s="426" t="s">
+      <c r="F48" s="429" t="s">
         <v>229</v>
       </c>
-      <c r="G48" s="427"/>
+      <c r="G48" s="430"/>
       <c r="H48" s="128" t="e">
         <f>I48/(I48+I54)</f>
         <v>#DIV/0!</v>
@@ -56792,10 +56799,10 @@
         <f>CV_C!I29</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F50" s="426" t="s">
+      <c r="F50" s="429" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="427"/>
+      <c r="G50" s="430"/>
       <c r="H50" s="243" t="s">
         <v>231</v>
       </c>
@@ -56819,10 +56826,10 @@
         <f>CV_C!I30</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F51" s="426" t="s">
+      <c r="F51" s="429" t="s">
         <v>232</v>
       </c>
-      <c r="G51" s="427"/>
+      <c r="G51" s="430"/>
       <c r="H51" s="128" t="e">
         <f>I51/(I51+I57)</f>
         <v>#DIV/0!</v>
@@ -56873,10 +56880,10 @@
         <f>CV_C!I32</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F53" s="426" t="s">
+      <c r="F53" s="429" t="s">
         <v>233</v>
       </c>
-      <c r="G53" s="427"/>
+      <c r="G53" s="430"/>
       <c r="H53" s="243" t="s">
         <v>228</v>
       </c>
@@ -56900,10 +56907,10 @@
         <f>CV_C!I33</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F54" s="426" t="s">
+      <c r="F54" s="429" t="s">
         <v>229</v>
       </c>
-      <c r="G54" s="427"/>
+      <c r="G54" s="430"/>
       <c r="H54" s="128" t="e">
         <f>I54/(I54+I48)</f>
         <v>#DIV/0!</v>
@@ -56954,10 +56961,10 @@
         <f>CV_C!I35</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F56" s="426" t="s">
+      <c r="F56" s="429" t="s">
         <v>234</v>
       </c>
-      <c r="G56" s="433"/>
+      <c r="G56" s="436"/>
       <c r="H56" s="243" t="s">
         <v>231</v>
       </c>
@@ -56981,10 +56988,10 @@
         <f>CV_C!I36</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F57" s="426" t="s">
+      <c r="F57" s="429" t="s">
         <v>232</v>
       </c>
-      <c r="G57" s="433"/>
+      <c r="G57" s="436"/>
       <c r="H57" s="128" t="e">
         <f>I57/(I57+I51)</f>
         <v>#DIV/0!</v>
@@ -57167,27 +57174,27 @@
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
-      <c r="C9" s="430" t="str">
+      <c r="C9" s="433" t="str">
         <f>CV_H!C10</f>
         <v>Tous Véhicules</v>
       </c>
-      <c r="D9" s="430"/>
-      <c r="E9" s="430"/>
-      <c r="F9" s="431" t="str">
+      <c r="D9" s="433"/>
+      <c r="E9" s="433"/>
+      <c r="F9" s="434" t="str">
         <f>CV_H!F10</f>
         <v>Véhicules légers</v>
       </c>
-      <c r="G9" s="431"/>
-      <c r="H9" s="432" t="str">
+      <c r="G9" s="434"/>
+      <c r="H9" s="435" t="str">
         <f>CV_H!H10</f>
         <v>Poids lourds</v>
       </c>
-      <c r="I9" s="432"/>
-      <c r="J9" s="423" t="str">
+      <c r="I9" s="435"/>
+      <c r="J9" s="426" t="str">
         <f>CV_H!J10</f>
         <v>% Poids lourds</v>
       </c>
-      <c r="K9" s="423"/>
+      <c r="K9" s="426"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
@@ -57305,27 +57312,27 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="425" t="s">
+      <c r="A14" s="428" t="s">
         <v>222</v>
       </c>
-      <c r="B14" s="425"/>
-      <c r="C14" s="425"/>
-      <c r="D14" s="425"/>
-      <c r="E14" s="425"/>
-      <c r="F14" s="425"/>
-      <c r="G14" s="425"/>
-      <c r="H14" s="425"/>
-      <c r="I14" s="425"/>
-      <c r="J14" s="425"/>
-      <c r="K14" s="425"/>
+      <c r="B14" s="428"/>
+      <c r="C14" s="428"/>
+      <c r="D14" s="428"/>
+      <c r="E14" s="428"/>
+      <c r="F14" s="428"/>
+      <c r="G14" s="428"/>
+      <c r="H14" s="428"/>
+      <c r="I14" s="428"/>
+      <c r="J14" s="428"/>
+      <c r="K14" s="428"/>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="424" t="s">
+      <c r="A33" s="427" t="s">
         <v>203</v>
       </c>
-      <c r="B33" s="424"/>
-      <c r="C33" s="424"/>
-      <c r="D33" s="424"/>
+      <c r="B33" s="427"/>
+      <c r="C33" s="427"/>
+      <c r="D33" s="427"/>
       <c r="E33" s="39"/>
       <c r="F33"/>
       <c r="G33"/>

</xml_diff>